<commit_message>
Position control updated to account for change in direction
</commit_message>
<xml_diff>
--- a/4_Paddle_Controller/1_Electrical/FIT0493_Motor_wEncoder/Speed_Calcs.xlsx
+++ b/4_Paddle_Controller/1_Electrical/FIT0493_Motor_wEncoder/Speed_Calcs.xlsx
@@ -393,7 +393,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,7 +430,7 @@
         <v>374</v>
       </c>
       <c r="D2">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -496,7 +496,7 @@
       </c>
       <c r="D8">
         <f>C8*D2/60</f>
-        <v>113.77858686995108</v>
+        <v>341.33576060985325</v>
       </c>
       <c r="F8">
         <v>10</v>

</xml_diff>